<commit_message>
Usando o classificador na base de teste, verificando os percentusias de acerto e erro.
</commit_message>
<xml_diff>
--- a/cocacola.xlsx
+++ b/cocacola.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f108549a37e245cb/Área de Trabalho/Ciencia dos Dados/P1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f108549a37e245cb/Área de Trabalho/Ciencia dos Dados/P1/TweetsClassifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{1731F555-1BAC-4001-93B0-BA06364703A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{48F845FC-75D1-4D1C-BFA9-95070F5C895C}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{1731F555-1BAC-4001-93B0-BA06364703A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2B30114-3586-478E-B6F2-D6548771E78A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="573">
   <si>
     <t>Treinamento</t>
   </si>
@@ -5529,8 +5529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B190" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5542,6 +5542,9 @@
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
+      <c r="B1" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -7149,21 +7152,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4840AA19C5BB345B207E7F500E224CA" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="06ea5bef7740b623339648500d8f8038">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="129a5b91-8fe4-4dde-8e8f-bb793fbb3f5e" xmlns:ns4="bf71c534-09aa-48fe-acbf-3d088c7a3ff7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62dd8e2fd97c58f7354f6218effb4af9" ns3:_="" ns4:_="">
     <xsd:import namespace="129a5b91-8fe4-4dde-8e8f-bb793fbb3f5e"/>
@@ -7386,10 +7374,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D924C47-2B1C-4A71-892F-03C29D3E00B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AE91881-018D-4D44-B4DC-67C235AD5960}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="129a5b91-8fe4-4dde-8e8f-bb793fbb3f5e"/>
+    <ds:schemaRef ds:uri="bf71c534-09aa-48fe-acbf-3d088c7a3ff7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7412,20 +7426,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AE91881-018D-4D44-B4DC-67C235AD5960}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D924C47-2B1C-4A71-892F-03C29D3E00B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="129a5b91-8fe4-4dde-8e8f-bb793fbb3f5e"/>
-    <ds:schemaRef ds:uri="bf71c534-09aa-48fe-acbf-3d088c7a3ff7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>